<commit_message>
update manual cases; add libs tips
</commit_message>
<xml_diff>
--- a/test_cases_backbase.xlsx
+++ b/test_cases_backbase.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="176">
   <si>
     <t xml:space="preserve">Functionality </t>
   </si>
@@ -145,9 +145,6 @@
     <t>Delete computer</t>
   </si>
   <si>
-    <t>In general filter could be more interactive (instead of forsing a user to click the button). E.g. show options after user entered 3 symbols; refresh the table after user cleared the field</t>
-  </si>
-  <si>
     <t> Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silver Rocket  Silv</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>Computer name link</t>
   </si>
   <si>
-    <t>AN/FSQ-32</t>
-  </si>
-  <si>
     <t>Edit computer page is opened</t>
   </si>
   <si>
@@ -466,9 +460,6 @@
     <t>1 test computer 1</t>
   </si>
   <si>
-    <t>Success message is shown; the cumputer is NOT in the table</t>
-  </si>
-  <si>
     <t>Click '1 test computer ' in the table</t>
   </si>
   <si>
@@ -490,9 +481,6 @@
     <t>Success message is shown;all fields are updated correctly</t>
   </si>
   <si>
-    <t>Recommended to automate</t>
-  </si>
-  <si>
     <t>Cancel creation</t>
   </si>
   <si>
@@ -532,6 +520,12 @@
     <t>Check that functionality is the same in Edge</t>
   </si>
   <si>
+    <t>In general filter could be more interactive (instead of forcing a user to click the button). E.g. show options after user entered 3 symbols; refresh the table after user cleared the field</t>
+  </si>
+  <si>
+    <t>The field shouldn't allow a value longer than reasonable length. Error message should be displayed as well</t>
+  </si>
+  <si>
     <t>Success message is shown; the computer is in the table; header is "575 computers found"</t>
   </si>
   <si>
@@ -551,6 +545,12 @@
   </si>
   <si>
     <t>APEX</t>
+  </si>
+  <si>
+    <t>Partially</t>
+  </si>
+  <si>
+    <t>Success message is shown; the computer is NOT in the table</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1306,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1531,16 +1531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2049,8 +2040,8 @@
   <dimension ref="A1:AK60"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2070,7 +2061,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19" thickBot="1">
       <c r="A1" s="113" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>0</v>
@@ -2121,7 +2112,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2133,7 +2124,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>21</v>
@@ -2158,7 +2149,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>16</v>
@@ -2181,7 +2172,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>15</v>
@@ -2204,7 +2195,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" s="47" t="s">
         <v>29</v>
@@ -2248,10 +2239,10 @@
         <v>25</v>
       </c>
       <c r="D8" s="60" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="62" t="s">
         <v>26</v>
@@ -2271,20 +2262,20 @@
         <v>27</v>
       </c>
       <c r="D9" s="61" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" s="63" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="61"/>
       <c r="I9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16" thickBot="1"/>
@@ -2296,23 +2287,23 @@
         <v>5</v>
       </c>
       <c r="C11" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="50" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>49</v>
       </c>
       <c r="E11" s="57"/>
       <c r="F11" s="64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="53" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="57" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="I11" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16" thickBot="1">
@@ -2321,16 +2312,16 @@
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="61" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="F12" s="61" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>24</v>
@@ -2343,20 +2334,20 @@
     <row r="13" spans="1:9" ht="16" thickBot="1"/>
     <row r="14" spans="1:9" ht="30">
       <c r="A14" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="55" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="67" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>24</v>
@@ -2366,16 +2357,16 @@
     </row>
     <row r="15" spans="1:9" ht="30">
       <c r="A15" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="30"/>
       <c r="D15" s="58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="68" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>24</v>
@@ -2385,16 +2376,16 @@
     </row>
     <row r="16" spans="1:9" ht="30">
       <c r="A16" s="71" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="31"/>
       <c r="D16" s="60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G16" s="34" t="s">
         <v>24</v>
@@ -2404,20 +2395,20 @@
     </row>
     <row r="17" spans="1:9" ht="30">
       <c r="A17" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="66" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E17" s="38" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="70" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G17" s="40" t="s">
         <v>24</v>
@@ -2429,16 +2420,16 @@
     </row>
     <row r="18" spans="1:9" ht="45">
       <c r="A18" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="30"/>
       <c r="D18" s="58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="68" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>28</v>
@@ -2447,21 +2438,21 @@
         <v>24</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30">
       <c r="A19" s="71" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="31"/>
       <c r="D19" s="60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="69" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G19" s="34" t="s">
         <v>24</v>
@@ -2477,16 +2468,16 @@
       </c>
       <c r="B20" s="56"/>
       <c r="C20" s="26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>24</v>
@@ -2497,20 +2488,20 @@
     <row r="21" spans="1:9" ht="16" thickBot="1"/>
     <row r="22" spans="1:9">
       <c r="A22" s="20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B22" s="55" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="77" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22" s="65"/>
       <c r="F22" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G22" s="85" t="s">
         <v>24</v>
@@ -2522,18 +2513,18 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="78"/>
       <c r="D23" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F23" s="73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G23" s="86" t="s">
         <v>24</v>
@@ -2545,18 +2536,18 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="78"/>
       <c r="D24" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E24" s="82" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G24" s="86" t="s">
         <v>24</v>
@@ -2568,18 +2559,18 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="78"/>
       <c r="D25" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E25" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="73" t="s">
         <v>101</v>
-      </c>
-      <c r="F25" s="73" t="s">
-        <v>103</v>
       </c>
       <c r="G25" s="86" t="s">
         <v>24</v>
@@ -2591,18 +2582,18 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B26" s="28"/>
       <c r="C26" s="78"/>
       <c r="D26" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F26" s="73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G26" s="86" t="s">
         <v>24</v>
@@ -2614,16 +2605,16 @@
     </row>
     <row r="27" spans="1:9" ht="45">
       <c r="A27" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="78"/>
       <c r="D27" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E27" s="58"/>
       <c r="F27" s="73" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G27" s="86" t="s">
         <v>24</v>
@@ -2635,18 +2626,18 @@
     </row>
     <row r="28" spans="1:9" ht="30">
       <c r="A28" s="76" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="79"/>
       <c r="D28" s="32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E28" s="60" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F28" s="74" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G28" s="87" t="s">
         <v>24</v>
@@ -2658,18 +2649,18 @@
     </row>
     <row r="29" spans="1:9" ht="30">
       <c r="A29" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="80" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E29" s="66"/>
       <c r="F29" s="75" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G29" s="88" t="s">
         <v>24</v>
@@ -2678,42 +2669,42 @@
         <v>24</v>
       </c>
       <c r="I29" s="94" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30">
       <c r="A30" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B30" s="28"/>
       <c r="C30" s="78"/>
       <c r="D30" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E30" s="58"/>
       <c r="F30" s="73" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G30" s="86" t="s">
         <v>24</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="95" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30">
       <c r="A31" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31" s="28"/>
       <c r="C31" s="78"/>
       <c r="D31" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E31" s="58"/>
       <c r="F31" s="73" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G31" s="86" t="s">
         <v>24</v>
@@ -2723,16 +2714,16 @@
     </row>
     <row r="32" spans="1:9" ht="30">
       <c r="A32" s="76" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="79"/>
       <c r="D32" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32" s="60"/>
       <c r="F32" s="74" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G32" s="87" t="s">
         <v>24</v>
@@ -2742,32 +2733,32 @@
     </row>
     <row r="33" spans="1:9" ht="30">
       <c r="A33" s="21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B33" s="28"/>
       <c r="C33" s="80" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E33" s="117" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="F33" s="75" t="s">
-        <v>110</v>
-      </c>
       <c r="G33" s="118" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H33" s="37"/>
       <c r="I33" s="119" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="45">
       <c r="A34" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B34" s="28"/>
       <c r="C34" s="78"/>
@@ -2775,56 +2766,56 @@
         <v>27</v>
       </c>
       <c r="E34" s="68" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G34" s="90" t="s">
         <v>28</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="97" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="45">
       <c r="A35" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="78"/>
       <c r="D35" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F35" s="73" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G35" s="90" t="s">
         <v>28</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="97" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30">
       <c r="A36" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="78"/>
       <c r="D36" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F36" s="73" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G36" s="86" t="s">
         <v>24</v>
@@ -2834,18 +2825,18 @@
     </row>
     <row r="37" spans="1:9" ht="30">
       <c r="A37" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="78"/>
       <c r="D37" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E37" s="68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F37" s="73" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G37" s="86" t="s">
         <v>24</v>
@@ -2855,41 +2846,41 @@
     </row>
     <row r="38" spans="1:9" ht="30">
       <c r="A38" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B38" s="28"/>
       <c r="C38" s="78"/>
       <c r="D38" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E38" s="83" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G38" s="89" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="98" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30">
       <c r="A39" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B39" s="28"/>
       <c r="C39" s="78"/>
       <c r="D39" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E39" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" s="22" t="s">
         <v>116</v>
-      </c>
-      <c r="F39" s="22" t="s">
-        <v>118</v>
       </c>
       <c r="G39" s="86" t="s">
         <v>24</v>
@@ -2899,18 +2890,18 @@
     </row>
     <row r="40" spans="1:9" ht="30">
       <c r="A40" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B40" s="28"/>
       <c r="C40" s="78"/>
       <c r="D40" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E40" s="68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G40" s="86" t="s">
         <v>24</v>
@@ -2923,36 +2914,36 @@
       <c r="B41" s="28"/>
       <c r="C41" s="79"/>
       <c r="D41" s="33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E41" s="69" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F41" s="33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G41" s="120" t="s">
         <v>28</v>
       </c>
       <c r="H41" s="32"/>
       <c r="I41" s="121" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="31" thickBot="1">
       <c r="A42" s="25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B42" s="56"/>
       <c r="C42" s="116" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E42" s="84"/>
       <c r="F42" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G42" s="111" t="s">
         <v>24</v>
@@ -2969,14 +2960,14 @@
         <v>38</v>
       </c>
       <c r="C44" s="77" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E44" s="65"/>
       <c r="F44" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G44" s="85" t="s">
         <v>24</v>
@@ -2993,13 +2984,13 @@
       <c r="B45" s="28"/>
       <c r="C45" s="78"/>
       <c r="D45" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F45" s="73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G45" s="86" t="s">
         <v>24</v>
@@ -3016,13 +3007,13 @@
       <c r="B46" s="28"/>
       <c r="C46" s="78"/>
       <c r="D46" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E46" s="82" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F46" s="73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G46" s="86" t="s">
         <v>24</v>
@@ -3039,13 +3030,13 @@
       <c r="B47" s="28"/>
       <c r="C47" s="78"/>
       <c r="D47" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E47" s="82" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F47" s="73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G47" s="86" t="s">
         <v>24</v>
@@ -3062,13 +3053,13 @@
       <c r="B48" s="28"/>
       <c r="C48" s="78"/>
       <c r="D48" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E48" s="58" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F48" s="73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G48" s="86" t="s">
         <v>24</v>
@@ -3085,11 +3076,11 @@
       <c r="B49" s="56"/>
       <c r="C49" s="81"/>
       <c r="D49" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E49" s="61"/>
       <c r="F49" s="110" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G49" s="111" t="s">
         <v>24</v>
@@ -3111,11 +3102,11 @@
       </c>
       <c r="C51" s="50"/>
       <c r="D51" s="108" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E51" s="50"/>
       <c r="F51" s="107" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="G51" s="51" t="s">
         <v>24</v>
@@ -3130,10 +3121,10 @@
       <c r="B52" s="56"/>
       <c r="C52" s="10"/>
       <c r="D52" s="61" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F52" s="84" t="s">
         <v>26</v>
@@ -3141,7 +3132,9 @@
       <c r="G52" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="61"/>
+      <c r="H52" s="61" t="s">
+        <v>24</v>
+      </c>
       <c r="I52" s="16"/>
     </row>
     <row r="53" spans="1:37" ht="16" thickBot="1">
@@ -3184,19 +3177,19 @@
         <v>8</v>
       </c>
       <c r="B56" s="109" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="122" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" s="123" t="s">
+        <v>158</v>
+      </c>
+      <c r="E56" s="101" t="s">
         <v>160</v>
       </c>
-      <c r="C56" s="122" t="s">
-        <v>161</v>
-      </c>
-      <c r="D56" s="123" t="s">
-        <v>162</v>
-      </c>
-      <c r="E56" s="101" t="s">
-        <v>164</v>
-      </c>
       <c r="F56" s="106" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G56" s="102" t="s">
         <v>24</v>
@@ -3209,18 +3202,18 @@
       <c r="A58" s="105">
         <v>9</v>
       </c>
-      <c r="B58" s="125" t="s">
-        <v>174</v>
+      <c r="B58" s="55" t="s">
+        <v>172</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D58" s="64" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E58" s="50"/>
       <c r="F58" s="57" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G58" s="51" t="s">
         <v>24</v>
@@ -3257,24 +3250,24 @@
       <c r="AK58"/>
     </row>
     <row r="59" spans="1:37" s="47" customFormat="1" ht="30">
-      <c r="A59" s="126">
+      <c r="A59" s="124">
         <v>9.1</v>
       </c>
-      <c r="B59" s="127"/>
-      <c r="C59" s="128" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59" s="129" t="s">
-        <v>166</v>
+      <c r="B59" s="28"/>
+      <c r="C59" s="125" t="s">
+        <v>163</v>
+      </c>
+      <c r="D59" s="126" t="s">
+        <v>162</v>
       </c>
       <c r="F59" s="59" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G59" s="48" t="s">
         <v>24</v>
       </c>
       <c r="H59" s="59"/>
-      <c r="I59" s="130"/>
+      <c r="I59" s="127"/>
       <c r="J59"/>
       <c r="K59"/>
       <c r="L59"/>
@@ -3308,16 +3301,16 @@
       <c r="A60" s="25">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B60" s="124"/>
+      <c r="B60" s="56"/>
       <c r="C60" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D60" s="63" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="61" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G60" s="15" t="s">
         <v>24</v>
@@ -3326,7 +3319,8 @@
       <c r="I60" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="B58:B60"/>
     <mergeCell ref="C29:C32"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="I30:I32"/>
@@ -3368,7 +3362,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="409">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3394,22 +3388,22 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
@@ -3417,7 +3411,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>